<commit_message>
fix bug Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_ホワイトボート_トラブル一覧.xlsx
+++ b/test_物件管理/test_ホワイトボート_トラブル一覧.xlsx
@@ -3563,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:KP147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3764,7 +3764,7 @@
       <c r="A24" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="196" t="s">
         <v>486</v>
       </c>
     </row>

</xml_diff>